<commit_message>
added mongo data with new excel file
</commit_message>
<xml_diff>
--- a/server/LMS.xlsx
+++ b/server/LMS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qasim/NodeJs/renovationUpdates/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFA9615C-7206-CA41-90EF-9E305EE48373}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E47E761-612C-FF4A-B71F-89C4CF894345}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{DA0D76AD-D22C-F94B-BEC5-B33AAC6C9115}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>Rank</t>
   </si>
@@ -33,9 +33,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Addl Days</t>
-  </si>
-  <si>
     <t>P Lve</t>
   </si>
   <si>
@@ -48,52 +45,55 @@
     <t>No</t>
   </si>
   <si>
-    <t>Leave</t>
-  </si>
-  <si>
     <t>Akram Khan</t>
   </si>
   <si>
     <t>Ilyas Hussain</t>
   </si>
   <si>
-    <t>type: C;
-starts: 2 Nov 2019;
-ends: 16 Nov 2019;
-bonus: 0;</t>
-  </si>
-  <si>
     <t>Rafi Ullah</t>
   </si>
   <si>
-    <t>type: C;
-starts: 10 Sep 2019;
-ends: 23 Sep 2019;
-bonus: -2;</t>
-  </si>
-  <si>
-    <t>type: C;
-starts: 1 Oct 2019;
-ends: 11 Oct 2019;
-bonus: -2;</t>
-  </si>
-  <si>
-    <t>type: W1;
-starts: 12 Dec 2019;
-ends: 17 Dec 2019;
-bonus: 4;</t>
-  </si>
-  <si>
-    <t>type: W1;
-starts: 24 Dec 2019;
-ends: 30 Dec 2019;
-bonus: 4;</t>
-  </si>
-  <si>
-    <t>type: W2;
-starts: 12 Jan 2020;
-ends: 14 Jan 2020;
-bonus: 0;</t>
+    <t>addlDays</t>
+  </si>
+  <si>
+    <t>leave</t>
+  </si>
+  <si>
+    <t>leaveType: C;
+start: 1 Oct 2019;
+end: 11 Oct 2019;
+specialDays: -2;</t>
+  </si>
+  <si>
+    <t>leaveType: W1;
+start: 12 Dec 2019;
+end: 17 Dec 2019;
+specialDays: 4;</t>
+  </si>
+  <si>
+    <t>leaveType: W2;
+start: 12 Jan 2020;
+end: 14 Jan 2020;
+specialDays: 0;</t>
+  </si>
+  <si>
+    <t>leaveType: C;
+start: 10 Sep 2019;
+end: 23 Sep 2019;
+specialDays: -2;</t>
+  </si>
+  <si>
+    <t>leaveType: W1;
+start: 24 Dec 2019;
+end: 30 Dec 2019;
+specialDays: 4;</t>
+  </si>
+  <si>
+    <t>leaveType: C;
+start: 2 Nov 2019;
+end: 16 Nov 2019;
+specialDays: 0;</t>
   </si>
 </sst>
 </file>
@@ -485,7 +485,7 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -502,7 +502,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -511,27 +511,27 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="76" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D2" s="5">
         <v>0</v>
@@ -540,21 +540,21 @@
         <v>43497</v>
       </c>
       <c r="F2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>13</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="76" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D3" s="5">
         <v>2</v>
@@ -563,7 +563,7 @@
         <v>43525</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>15</v>
@@ -572,10 +572,10 @@
     </row>
     <row r="4" spans="1:8" ht="76" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D4" s="5">
         <v>0</v>
@@ -584,11 +584,9 @@
         <v>43770</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>15</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="G4" s="8"/>
       <c r="H4" s="8"/>
     </row>
     <row r="5" spans="1:8" ht="18" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
calculate fwd and back distances
</commit_message>
<xml_diff>
--- a/server/LMS.xlsx
+++ b/server/LMS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/QasimAli/nodejs/renovationUpdates/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AEAFF10-3494-2D44-B1A8-443DB28C3A7D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F37031CA-9F95-3D44-B23C-C2CCBA7C72EB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="18000" xr2:uid="{DA0D76AD-D22C-F94B-BEC5-B33AAC6C9115}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>Rank</t>
   </si>
@@ -100,6 +100,12 @@
 start: 22 Dec 2019;
 end: 29 Dec 2019;
 specialDays: 4;</t>
+  </si>
+  <si>
+    <t>leaveType:C;
+start: 12 Feb 2020;
+end: 24 Feb 2020;
+specialDays: -1;</t>
   </si>
 </sst>
 </file>
@@ -488,10 +494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25FC75BF-6045-8448-8FF0-6EFD59B34696}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -503,10 +509,11 @@
     <col min="5" max="5" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="22.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="23.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="2"/>
+    <col min="9" max="9" width="21.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -531,8 +538,11 @@
       <c r="H1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="76" x14ac:dyDescent="0.2">
+      <c r="I1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="95" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
@@ -554,8 +564,11 @@
       <c r="H2" s="8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="76" x14ac:dyDescent="0.2">
+      <c r="I2" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="76" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
@@ -576,7 +589,7 @@
       </c>
       <c r="H3" s="8"/>
     </row>
-    <row r="4" spans="1:8" ht="76" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="76" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
@@ -597,7 +610,7 @@
       </c>
       <c r="H4" s="8"/>
     </row>
-    <row r="5" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="B5" s="3"/>
       <c r="C5" s="4"/>
       <c r="D5" s="5"/>
@@ -605,7 +618,7 @@
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
     </row>
-    <row r="6" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="B6" s="3"/>
       <c r="C6" s="4"/>
       <c r="D6" s="5"/>
@@ -613,7 +626,7 @@
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
     </row>
-    <row r="7" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="B7" s="3"/>
       <c r="C7" s="4"/>
       <c r="D7" s="5"/>
@@ -621,7 +634,7 @@
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="B8" s="3"/>
       <c r="C8" s="4"/>
       <c r="D8" s="5"/>
@@ -629,7 +642,7 @@
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
     </row>
-    <row r="9" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="B9" s="3"/>
       <c r="C9" s="4"/>
       <c r="D9" s="5"/>
@@ -637,7 +650,7 @@
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
     </row>
-    <row r="10" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="B10" s="3"/>
       <c r="C10" s="4"/>
       <c r="D10" s="5"/>
@@ -645,7 +658,7 @@
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
     </row>
-    <row r="11" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="B11" s="3"/>
       <c r="C11" s="4"/>
       <c r="D11" s="5"/>
@@ -653,7 +666,7 @@
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
     </row>
-    <row r="12" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="B12" s="3"/>
       <c r="C12" s="4"/>
       <c r="D12" s="5"/>
@@ -661,7 +674,7 @@
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
     </row>
-    <row r="13" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="B13" s="3"/>
       <c r="C13" s="4"/>
       <c r="D13" s="5"/>
@@ -669,7 +682,7 @@
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
     </row>
-    <row r="14" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="B14" s="3"/>
       <c r="C14" s="4"/>
       <c r="D14" s="5"/>
@@ -677,7 +690,7 @@
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
     </row>
-    <row r="15" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="B15" s="3"/>
       <c r="C15" s="4"/>
       <c r="D15" s="5"/>
@@ -685,7 +698,7 @@
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:8" ht="18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="18" x14ac:dyDescent="0.2">
       <c r="B16" s="3"/>
       <c r="C16" s="4"/>
       <c r="D16" s="5"/>

</xml_diff>

<commit_message>
fixed leave issue where c lve was being rptd
</commit_message>
<xml_diff>
--- a/server/LMS.xlsx
+++ b/server/LMS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/QasimAli/nodejs/renovationUpdates/server/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qasim/NodeJs/renovationUpdates/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F37031CA-9F95-3D44-B23C-C2CCBA7C72EB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{169D8705-D599-5C42-94A8-CAA17ACF34A8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="18000" xr2:uid="{DA0D76AD-D22C-F94B-BEC5-B33AAC6C9115}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16740" xr2:uid="{DA0D76AD-D22C-F94B-BEC5-B33AAC6C9115}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>Rank</t>
   </si>
@@ -66,12 +66,6 @@
 specialDays: -2;</t>
   </si>
   <si>
-    <t>leaveType: W1;
-start: 12 Dec 2019;
-end: 17 Dec 2019;
-specialDays: 4;</t>
-  </si>
-  <si>
     <t>leaveType: W2;
 start: 12 Jan 2020;
 end: 14 Jan 2020;
@@ -84,12 +78,6 @@
 specialDays: -2;</t>
   </si>
   <si>
-    <t>leaveType: W1;
-start: 24 Dec 2019;
-end: 30 Dec 2019;
-specialDays: 4;</t>
-  </si>
-  <si>
     <t>leaveType: C;
 start: 2 Nov 2019;
 end: 16 Nov 2019;
@@ -106,6 +94,42 @@
 start: 12 Feb 2020;
 end: 24 Feb 2020;
 specialDays: -1;</t>
+  </si>
+  <si>
+    <t>leaveType: W1;
+start: 4 Nov 2019;
+end: 11 Nov 2019;
+specialDays: 4;</t>
+  </si>
+  <si>
+    <t>leaveType: W1;
+start: 11 Nov 2019;
+end: 15 Nov 2019;
+specialDays: 4;</t>
+  </si>
+  <si>
+    <t>leaveType: W2;
+start: 1 Nov 2019;
+end: 2 Nov 2019;
+specialDays: 0;</t>
+  </si>
+  <si>
+    <t>leaveType: C;
+start: 5 Dec 2019;
+end: 18 Dec 2019;
+specialDays: 0;</t>
+  </si>
+  <si>
+    <t>leaveType: W1;
+start: 18 Jan 2019;
+end: 21 Jan 2019;
+specialDays: 0;</t>
+  </si>
+  <si>
+    <t>Hav</t>
+  </si>
+  <si>
+    <t>Hashim</t>
   </si>
 </sst>
 </file>
@@ -154,7 +178,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -179,6 +203,15 @@
     </xf>
     <xf numFmtId="15" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -494,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25FC75BF-6045-8448-8FF0-6EFD59B34696}">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -505,15 +538,18 @@
     <col min="1" max="1" width="3.5" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.33203125" style="2" customWidth="1"/>
     <col min="5" max="5" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="22.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="23.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21.1640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="10.83203125" style="2"/>
+    <col min="10" max="11" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="2.5" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -542,7 +578,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="95" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="95" x14ac:dyDescent="0.2">
       <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
@@ -559,16 +595,16 @@
         <v>11</v>
       </c>
       <c r="G2" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="8" t="s">
-        <v>13</v>
-      </c>
       <c r="I2" s="8" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="76" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="76" x14ac:dyDescent="0.2">
       <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
@@ -582,14 +618,18 @@
         <v>43525</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H3" s="8"/>
-    </row>
-    <row r="4" spans="1:9" ht="76" x14ac:dyDescent="0.2">
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="11"/>
+    </row>
+    <row r="4" spans="1:13" ht="76" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
@@ -603,148 +643,241 @@
         <v>43770</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H4" s="8"/>
-    </row>
-    <row r="5" spans="1:9" ht="18" x14ac:dyDescent="0.2">
-      <c r="B5" s="3"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-    </row>
-    <row r="6" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="J4" s="9"/>
+      <c r="K4" s="9"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="11"/>
+    </row>
+    <row r="5" spans="1:13" ht="76" x14ac:dyDescent="0.2">
+      <c r="B5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="5">
+        <v>2</v>
+      </c>
+      <c r="E5" s="6">
+        <v>44013</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" s="9"/>
+      <c r="K5" s="9"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="11"/>
+    </row>
+    <row r="6" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="B6" s="3"/>
       <c r="C6" s="4"/>
       <c r="D6" s="5"/>
       <c r="E6" s="6"/>
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
-    </row>
-    <row r="7" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="11"/>
+    </row>
+    <row r="7" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="B7" s="3"/>
       <c r="C7" s="4"/>
       <c r="D7" s="5"/>
       <c r="E7" s="6"/>
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
-    </row>
-    <row r="8" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="J7" s="9"/>
+      <c r="K7" s="9"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="11"/>
+    </row>
+    <row r="8" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="B8" s="3"/>
       <c r="C8" s="4"/>
       <c r="D8" s="5"/>
       <c r="E8" s="6"/>
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
-    </row>
-    <row r="9" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="11"/>
+    </row>
+    <row r="9" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="B9" s="3"/>
       <c r="C9" s="4"/>
       <c r="D9" s="5"/>
       <c r="E9" s="6"/>
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
-    </row>
-    <row r="10" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="11"/>
+    </row>
+    <row r="10" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="B10" s="3"/>
       <c r="C10" s="4"/>
       <c r="D10" s="5"/>
       <c r="E10" s="6"/>
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
-    </row>
-    <row r="11" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="11"/>
+    </row>
+    <row r="11" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="B11" s="3"/>
       <c r="C11" s="4"/>
       <c r="D11" s="5"/>
       <c r="E11" s="6"/>
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
-    </row>
-    <row r="12" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="11"/>
+    </row>
+    <row r="12" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="B12" s="3"/>
       <c r="C12" s="4"/>
       <c r="D12" s="5"/>
       <c r="E12" s="6"/>
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
-    </row>
-    <row r="13" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="11"/>
+    </row>
+    <row r="13" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="B13" s="3"/>
       <c r="C13" s="4"/>
       <c r="D13" s="5"/>
       <c r="E13" s="6"/>
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
-    </row>
-    <row r="14" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="11"/>
+    </row>
+    <row r="14" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="B14" s="3"/>
       <c r="C14" s="4"/>
       <c r="D14" s="5"/>
       <c r="E14" s="6"/>
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
-    </row>
-    <row r="15" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="11"/>
+    </row>
+    <row r="15" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="B15" s="3"/>
       <c r="C15" s="4"/>
       <c r="D15" s="5"/>
       <c r="E15" s="6"/>
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
-    </row>
-    <row r="16" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="11"/>
+    </row>
+    <row r="16" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="B16" s="3"/>
       <c r="C16" s="4"/>
       <c r="D16" s="5"/>
       <c r="E16" s="6"/>
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
-    </row>
-    <row r="17" spans="2:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="11"/>
+    </row>
+    <row r="17" spans="2:13" ht="18" x14ac:dyDescent="0.2">
       <c r="B17" s="3"/>
       <c r="C17" s="4"/>
       <c r="D17" s="5"/>
       <c r="E17" s="6"/>
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
-    </row>
-    <row r="18" spans="2:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="11"/>
+    </row>
+    <row r="18" spans="2:13" ht="18" x14ac:dyDescent="0.2">
       <c r="B18" s="3"/>
       <c r="C18" s="4"/>
       <c r="D18" s="5"/>
       <c r="E18" s="6"/>
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
-    </row>
-    <row r="19" spans="2:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="11"/>
+    </row>
+    <row r="19" spans="2:13" ht="18" x14ac:dyDescent="0.2">
       <c r="B19" s="3"/>
       <c r="C19" s="4"/>
       <c r="D19" s="5"/>
       <c r="E19" s="6"/>
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
-    </row>
-    <row r="20" spans="2:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="10"/>
+      <c r="M19" s="11"/>
+    </row>
+    <row r="20" spans="2:13" ht="18" x14ac:dyDescent="0.2">
       <c r="B20" s="3"/>
       <c r="C20" s="4"/>
       <c r="D20" s="5"/>
       <c r="E20" s="6"/>
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
-    </row>
-    <row r="21" spans="2:7" ht="18" x14ac:dyDescent="0.2">
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="11"/>
+    </row>
+    <row r="21" spans="2:13" ht="18" x14ac:dyDescent="0.2">
       <c r="B21" s="3"/>
       <c r="C21" s="4"/>
       <c r="D21" s="5"/>
       <c r="E21" s="6"/>
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="11"/>
+    </row>
+    <row r="22" spans="2:13" ht="18" x14ac:dyDescent="0.2">
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
saving progress for LMS
</commit_message>
<xml_diff>
--- a/server/LMS.xlsx
+++ b/server/LMS.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qasim/NodeJs/renovationUpdates/server/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF0EBACA-D4B5-3341-A364-A6E6FC41BE52}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A5F5093-E1C9-264B-9D9C-D28F3D5158DE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -875,7 +875,7 @@
     <xf numFmtId="15" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="17" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1195,8 +1195,8 @@
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H26" sqref="H26"/>
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2157,55 +2157,55 @@
       </c>
       <c r="I33" s="7"/>
     </row>
-    <row r="34" spans="1:9" s="13" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="8">
+    <row r="34" spans="1:9" s="17" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="7">
         <v>3702366</v>
       </c>
-      <c r="B34" s="9" t="s">
+      <c r="B34" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C34" s="9" t="s">
+      <c r="C34" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D34" s="8">
-        <v>0</v>
-      </c>
-      <c r="E34" s="10">
+      <c r="D34" s="7">
+        <v>0</v>
+      </c>
+      <c r="E34" s="6">
         <v>43878</v>
       </c>
-      <c r="F34" s="11" t="s">
+      <c r="F34" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="G34" s="11" t="s">
+      <c r="G34" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="H34" s="12"/>
-      <c r="I34" s="8"/>
-    </row>
-    <row r="35" spans="1:9" s="13" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="8">
+      <c r="H34" s="4"/>
+      <c r="I34" s="7"/>
+    </row>
+    <row r="35" spans="1:9" s="17" customFormat="1" ht="80" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="7">
         <v>3725050</v>
       </c>
-      <c r="B35" s="9" t="s">
+      <c r="B35" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C35" s="9" t="s">
+      <c r="C35" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D35" s="8">
+      <c r="D35" s="7">
         <v>0</v>
       </c>
       <c r="E35" s="21">
         <v>43862</v>
       </c>
-      <c r="F35" s="11" t="s">
+      <c r="F35" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="G35" s="11" t="s">
+      <c r="G35" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="H35" s="12"/>
-      <c r="I35" s="8"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>